<commit_message>
Added UI elements: Top bar showing (not yet connected) navigation buttons Bottom bar with surface / underground button (working)
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\OneDrive\Documents\Documents\4XCityBuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4848CDEC-417D-4B9D-A452-400D72E94B77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AAC57B-89CB-44BD-8036-80D72D35E4EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18315" windowHeight="12030" activeTab="1" xr2:uid="{A4CD2B52-042C-4D05-8156-D5CD0C816051}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -162,12 +162,6 @@
     <t>Fiber</t>
   </si>
   <si>
-    <t>Category 2</t>
-  </si>
-  <si>
-    <t>Category 1</t>
-  </si>
-  <si>
     <t>Tier 1</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
     <t>Dryad-Wood Bow</t>
   </si>
   <si>
-    <t>Specialty</t>
-  </si>
-  <si>
     <t>Butchering</t>
   </si>
   <si>
@@ -730,6 +721,36 @@
   </si>
   <si>
     <t>Adamantium Anvil</t>
+  </si>
+  <si>
+    <t>Class 1</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Class 2</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Healing Potion</t>
+  </si>
+  <si>
+    <t>Potion</t>
+  </si>
+  <si>
+    <t>Destruction</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>Explosive Arrow</t>
+  </si>
+  <si>
+    <t>Enchantment</t>
   </si>
 </sst>
 </file>
@@ -1112,11 +1133,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4C0326-3A5E-4D29-8D07-894863726E6A}">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,22 +1152,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>227</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
@@ -1157,16 +1178,16 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1174,16 +1195,16 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,16 +1212,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,16 +1229,16 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1225,10 +1246,10 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1242,10 +1263,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1259,10 +1280,10 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1276,10 +1297,10 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1293,10 +1314,10 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1316,22 +1337,22 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1339,22 +1360,22 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1362,22 +1383,22 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,7 +1406,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1394,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,7 +1423,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -1411,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1419,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1428,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1442,7 +1463,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1451,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,7 +1480,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1468,7 +1489,7 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1476,16 +1497,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,16 +1514,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1510,16 +1531,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,16 +1548,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
         <v>58</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,16 +1565,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1561,16 +1582,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1578,16 +1599,16 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1595,10 +1616,10 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1612,10 +1633,10 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1629,10 +1650,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -1646,16 +1667,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1663,16 +1684,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1680,16 +1701,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,16 +1718,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,16 +1735,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1731,7 +1752,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1754,7 +1775,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -1777,7 +1798,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -1800,7 +1821,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -1815,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,7 +1844,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -1843,683 +1864,683 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D42">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F42">
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
         <v>93</v>
-      </c>
-      <c r="D44">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D45">
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>233</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>131</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
         <v>128</v>
-      </c>
-      <c r="C47" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-      <c r="G47" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G49" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
         <v>134</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="G52" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G53" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G56" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G58" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>82</v>
-      </c>
-      <c r="F59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61">
+        <v>4</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D64">
-        <v>5</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="G64" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G67" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" t="s">
         <v>120</v>
       </c>
-      <c r="C68" t="s">
-        <v>123</v>
-      </c>
       <c r="D68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B69" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" t="s">
         <v>120</v>
       </c>
-      <c r="C69" t="s">
-        <v>123</v>
-      </c>
       <c r="D69">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G70" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G72" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G73" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G74" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C76" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G76" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2527,143 +2548,143 @@
         <v>90</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C78" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G78" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C79" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B80" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
         <v>19</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G82" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
       </c>
       <c r="D84">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G85" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -2672,49 +2693,49 @@
         <v>1</v>
       </c>
       <c r="G86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C87" t="s">
         <v>12</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
         <v>12</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C89" t="s">
         <v>12</v>
@@ -2723,987 +2744,987 @@
         <v>3</v>
       </c>
       <c r="G89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C90" t="s">
         <v>12</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G91" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
       </c>
       <c r="D94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
       </c>
       <c r="D95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D96">
         <v>5</v>
       </c>
       <c r="G96" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="B97" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="C97" t="s">
-        <v>225</v>
+        <v>19</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G97" t="s">
-        <v>226</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B98" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C98" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D98">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G98" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B99" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D99">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G99" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B100" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="C100" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="D100">
-        <v>1</v>
-      </c>
-      <c r="E100" t="s">
-        <v>172</v>
-      </c>
-      <c r="F100">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G100" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B101" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C101" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B102" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G102" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B103" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C103" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G103" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B104" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C104" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E104" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G104" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C105" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="F105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G105" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C106" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B107" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C107" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E107" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E108" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G108" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C109" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D109">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E109" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F109">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G109" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B110" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F110">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G110" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B112" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C112" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G112" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B113" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C113" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E113" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G113" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B114" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E114" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G114" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B115" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="C115" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E115" t="s">
+        <v>199</v>
+      </c>
+      <c r="F115">
+        <v>5</v>
       </c>
       <c r="G115" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B116" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C116" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B117" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C117" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G117" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C118" t="s">
+        <v>156</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+      <c r="G118" t="s">
         <v>159</v>
-      </c>
-      <c r="D118">
-        <v>4</v>
-      </c>
-      <c r="G118" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B119" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C119" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D119">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G119" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B120" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C120" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G120" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C121" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G121" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D122">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C123" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G123" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C124" t="s">
+        <v>150</v>
+      </c>
+      <c r="D124">
+        <v>4</v>
+      </c>
+      <c r="G124" t="s">
         <v>153</v>
-      </c>
-      <c r="D124">
-        <v>5</v>
-      </c>
-      <c r="G124" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C125" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="E125" t="s">
-        <v>172</v>
-      </c>
-      <c r="F125">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G125" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C126" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B127" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C127" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D127">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E127" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F127">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G127" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B128" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C128" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D128">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E128" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F128">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G128" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B129" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C129" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D129">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F129">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G129" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B130" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C130" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F130">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G130" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B131" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C131" t="s">
+        <v>180</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131" t="s">
         <v>183</v>
-      </c>
-      <c r="D131">
-        <v>2</v>
-      </c>
-      <c r="E131" t="s">
-        <v>172</v>
-      </c>
-      <c r="F131">
-        <v>2</v>
-      </c>
-      <c r="G131" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C132" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D132">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E132" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F132">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G132" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B133" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C133" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D133">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E133" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F133">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G133" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B134" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C134" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E134" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G134" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B135" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="C135" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E135" t="s">
+        <v>169</v>
+      </c>
+      <c r="F135">
+        <v>5</v>
       </c>
       <c r="G135" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>139</v>
+      </c>
+      <c r="C136" t="s">
         <v>141</v>
       </c>
-      <c r="B136" t="s">
-        <v>142</v>
-      </c>
-      <c r="C136" t="s">
-        <v>144</v>
-      </c>
       <c r="D136">
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" t="s">
+        <v>139</v>
+      </c>
+      <c r="C137" t="s">
         <v>141</v>
       </c>
-      <c r="B137" t="s">
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="G137" t="s">
         <v>142</v>
-      </c>
-      <c r="C137" t="s">
-        <v>144</v>
-      </c>
-      <c r="D137">
-        <v>2</v>
-      </c>
-      <c r="G137" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>139</v>
+      </c>
+      <c r="C138" t="s">
         <v>141</v>
       </c>
-      <c r="B138" t="s">
-        <v>142</v>
-      </c>
-      <c r="C138" t="s">
-        <v>144</v>
-      </c>
       <c r="D138">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G138" t="s">
         <v>147</v>
@@ -3711,50 +3732,50 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>139</v>
+      </c>
+      <c r="C139" t="s">
         <v>141</v>
       </c>
-      <c r="B139" t="s">
-        <v>142</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="D139">
+        <v>3</v>
+      </c>
+      <c r="G139" t="s">
         <v>144</v>
-      </c>
-      <c r="D139">
-        <v>4</v>
-      </c>
-      <c r="G139" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>139</v>
+      </c>
+      <c r="C140" t="s">
         <v>141</v>
       </c>
-      <c r="B140" t="s">
-        <v>142</v>
-      </c>
-      <c r="C140" t="s">
-        <v>144</v>
-      </c>
       <c r="D140">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G140" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>138</v>
+      </c>
+      <c r="B141" t="s">
+        <v>139</v>
+      </c>
+      <c r="C141" t="s">
         <v>141</v>
       </c>
-      <c r="B141" t="s">
-        <v>142</v>
-      </c>
-      <c r="C141" t="s">
-        <v>151</v>
-      </c>
       <c r="D141">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G141" t="s">
         <v>146</v>
@@ -3762,460 +3783,519 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C142" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D142">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G142" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C143" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D143">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G143" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B144" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C144" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G144" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C145" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D145">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G145" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C146" t="s">
+        <v>162</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+      <c r="G146" t="s">
         <v>165</v>
-      </c>
-      <c r="D146">
-        <v>4</v>
-      </c>
-      <c r="G146" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B147" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C147" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D147">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G147" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B148" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C148" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="D148">
-        <v>1</v>
-      </c>
-      <c r="E148" t="s">
-        <v>172</v>
-      </c>
-      <c r="F148">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G148" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B149" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C149" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E149" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G149" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B150" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C150" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D150">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E150" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F150">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G150" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B151" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C151" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D151">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E151" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F151">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G151" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C152" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D152">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E152" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F152">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G152" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B153" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
       <c r="C153" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E153" t="s">
+        <v>169</v>
+      </c>
+      <c r="F153">
+        <v>5</v>
       </c>
       <c r="G153" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B154" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C154" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D154">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G154" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B155" t="s">
+        <v>212</v>
+      </c>
+      <c r="C155" t="s">
+        <v>213</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="G155" t="s">
         <v>215</v>
-      </c>
-      <c r="C155" t="s">
-        <v>216</v>
-      </c>
-      <c r="D155">
-        <v>3</v>
-      </c>
-      <c r="G155" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C156" t="s">
+        <v>213</v>
+      </c>
+      <c r="D156">
+        <v>3</v>
+      </c>
+      <c r="G156" t="s">
         <v>216</v>
-      </c>
-      <c r="D156">
-        <v>4</v>
-      </c>
-      <c r="G156" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C157" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D157">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G157" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B158" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C158" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D158">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G158" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B159" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C159" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D159">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G159" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B160" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="C160" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="D160">
-        <v>1</v>
-      </c>
-      <c r="E160" t="s">
-        <v>202</v>
-      </c>
-      <c r="F160">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G160" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B161" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C161" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161" t="s">
+        <v>199</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+      <c r="G161" t="s">
         <v>202</v>
-      </c>
-      <c r="F161">
-        <v>2</v>
-      </c>
-      <c r="G161" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B162" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C162" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G162" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B163" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C163" t="s">
+        <v>201</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+      <c r="E163" t="s">
+        <v>199</v>
+      </c>
+      <c r="F163">
+        <v>3</v>
+      </c>
+      <c r="G163" t="s">
         <v>204</v>
-      </c>
-      <c r="D163">
-        <v>4</v>
-      </c>
-      <c r="E163" t="s">
-        <v>202</v>
-      </c>
-      <c r="F163">
-        <v>4</v>
-      </c>
-      <c r="G163" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B164" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C164" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D164">
+        <v>4</v>
+      </c>
+      <c r="E164" t="s">
+        <v>199</v>
+      </c>
+      <c r="F164">
+        <v>4</v>
+      </c>
+      <c r="G164" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>138</v>
+      </c>
+      <c r="B165" t="s">
+        <v>168</v>
+      </c>
+      <c r="C165" t="s">
+        <v>201</v>
+      </c>
+      <c r="D165">
         <v>5</v>
       </c>
-      <c r="E164" t="s">
-        <v>202</v>
-      </c>
-      <c r="F164">
+      <c r="E165" t="s">
+        <v>199</v>
+      </c>
+      <c r="F165">
         <v>5</v>
       </c>
-      <c r="G164" t="s">
-        <v>209</v>
+      <c r="G165" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>89</v>
+      </c>
+      <c r="B168" t="s">
+        <v>229</v>
+      </c>
+      <c r="C168" t="s">
+        <v>231</v>
+      </c>
+      <c r="D168">
+        <v>4</v>
+      </c>
+      <c r="G168" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>89</v>
+      </c>
+      <c r="B169" t="s">
+        <v>232</v>
+      </c>
+      <c r="C169" t="s">
+        <v>233</v>
+      </c>
+      <c r="D169">
+        <v>5</v>
+      </c>
+      <c r="G169" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>89</v>
+      </c>
+      <c r="B170" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G173">
-    <sortCondition ref="A2:A173"/>
-    <sortCondition ref="C2:C173"/>
-    <sortCondition ref="D2:D173"/>
+  <sortState ref="A2:G174">
+    <sortCondition ref="A2:A174"/>
+    <sortCondition ref="C2:C174"/>
+    <sortCondition ref="D2:D174"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished add, check, and remove resource methods Added resource table from Table Pro
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\OneDrive\Documents\Documents\4XCityBuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AAC57B-89CB-44BD-8036-80D72D35E4EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938FDD2-23C4-4C56-8429-5431FCE7839B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18315" windowHeight="12030" activeTab="1" xr2:uid="{A4CD2B52-042C-4D05-8156-D5CD0C816051}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="237">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Milk</t>
   </si>
   <si>
-    <t>Special mounts (special highest tier mount)</t>
-  </si>
-  <si>
     <t>Animal Husbandry</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
     <t>Ceramic Mugs</t>
   </si>
   <si>
-    <t>Base</t>
-  </si>
-  <si>
     <t>Earthworking</t>
   </si>
   <si>
@@ -723,15 +717,9 @@
     <t>Adamantium Anvil</t>
   </si>
   <si>
-    <t>Class 1</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Class 2</t>
-  </si>
-  <si>
     <t>Life</t>
   </si>
   <si>
@@ -751,6 +739,21 @@
   </si>
   <si>
     <t>Enchantment</t>
+  </si>
+  <si>
+    <t>Special mounts??</t>
+  </si>
+  <si>
+    <t>Enchanted Long Sword</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>Type 2</t>
   </si>
 </sst>
 </file>
@@ -1133,11 +1136,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4C0326-3A5E-4D29-8D07-894863726E6A}">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,24 +1150,24 @@
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -1178,10 +1181,10 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1195,10 +1198,10 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1212,16 +1215,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,16 +1232,16 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1246,10 +1249,10 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1263,10 +1266,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1280,10 +1283,10 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1297,10 +1300,10 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1314,10 +1317,10 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1337,22 +1340,22 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1360,22 +1363,22 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1383,22 +1386,22 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,7 +1409,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1415,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1423,7 +1426,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -1440,7 +1443,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1449,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1463,7 +1466,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1480,7 +1483,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1489,7 +1492,7 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1497,16 +1500,16 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1514,16 +1517,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
         <v>54</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1531,16 +1534,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1548,16 +1551,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1565,16 +1568,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
         <v>56</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1582,16 +1585,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1599,16 +1602,16 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1616,10 +1619,10 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1633,10 +1636,10 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1650,10 +1653,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -1667,16 +1670,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1684,16 +1687,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,16 +1704,16 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1718,10 +1721,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1735,16 +1738,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
-      <c r="G33" t="s">
-        <v>46</v>
+      <c r="G33" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1752,7 +1755,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1775,7 +1778,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -1798,7 +1801,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -1821,7 +1824,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -1836,7 +1839,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1844,7 +1847,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -1864,742 +1867,742 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
         <v>90</v>
-      </c>
-      <c r="B44" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
         <v>91</v>
-      </c>
-      <c r="D45">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>233</v>
+        <v>89</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G46" t="s">
-        <v>233</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" t="s">
         <v>125</v>
       </c>
-      <c r="C47" t="s">
-        <v>127</v>
-      </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
         <v>125</v>
-      </c>
-      <c r="C48" t="s">
-        <v>127</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
         <v>125</v>
       </c>
-      <c r="C49" t="s">
-        <v>127</v>
-      </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="G49" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D51">
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
         <v>132</v>
-      </c>
-      <c r="D52">
-        <v>5</v>
-      </c>
-      <c r="G52" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="G53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D54">
         <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D55">
         <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
         <v>117</v>
-      </c>
-      <c r="C56" t="s">
-        <v>119</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="G56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
         <v>117</v>
       </c>
-      <c r="C57" t="s">
-        <v>119</v>
-      </c>
       <c r="D57">
         <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
         <v>117</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="G58" t="s">
         <v>119</v>
-      </c>
-      <c r="D58">
-        <v>5</v>
-      </c>
-      <c r="G58" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F60">
         <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F61">
         <v>4</v>
       </c>
       <c r="G61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D63">
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D64">
         <v>4</v>
       </c>
       <c r="G64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D65">
         <v>5</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="G67" t="s">
         <v>80</v>
-      </c>
-      <c r="D67">
-        <v>3</v>
-      </c>
-      <c r="G67" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="G69" t="s">
         <v>120</v>
-      </c>
-      <c r="D69">
-        <v>3</v>
-      </c>
-      <c r="G69" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D70">
         <v>5</v>
       </c>
       <c r="G70" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="G71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D72">
         <v>3</v>
       </c>
       <c r="G72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C73" t="s">
+        <v>111</v>
+      </c>
+      <c r="D73">
+        <v>5</v>
+      </c>
+      <c r="G73" t="s">
         <v>113</v>
-      </c>
-      <c r="D73">
-        <v>5</v>
-      </c>
-      <c r="G73" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D74">
         <v>2</v>
       </c>
       <c r="G74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C75" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D75">
         <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D76">
         <v>5</v>
       </c>
       <c r="G76" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D77">
         <v>2</v>
       </c>
       <c r="G77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C78" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
         <v>76</v>
-      </c>
-      <c r="D78">
-        <v>3</v>
-      </c>
-      <c r="G78" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
         <v>19</v>
@@ -2613,10 +2616,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C82" t="s">
         <v>19</v>
@@ -2630,10 +2633,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -2647,10 +2650,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
@@ -2664,10 +2667,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
@@ -2681,10 +2684,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C86" t="s">
         <v>12</v>
@@ -2698,10 +2701,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
         <v>12</v>
@@ -2715,10 +2718,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C88" t="s">
         <v>12</v>
@@ -2732,10 +2735,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C89" t="s">
         <v>12</v>
@@ -2749,10 +2752,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
         <v>12</v>
@@ -2766,10 +2769,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C91" t="s">
         <v>12</v>
@@ -2783,10 +2786,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B92" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C92" t="s">
         <v>6</v>
@@ -2800,10 +2803,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
@@ -2817,10 +2820,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C94" t="s">
         <v>6</v>
@@ -2834,10 +2837,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C95" t="s">
         <v>6</v>
@@ -2851,10 +2854,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
@@ -2868,582 +2871,585 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B97" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="D97">
         <v>5</v>
       </c>
       <c r="G97" t="s">
-        <v>23</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C98" t="s">
-        <v>222</v>
+        <v>19</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G98" t="s">
-        <v>223</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="C99" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E99" t="s">
+        <v>167</v>
       </c>
       <c r="G99" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B100" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C100" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G100" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B101" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C101" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101" t="s">
-        <v>169</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G101" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C102" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="D102">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s">
-        <v>169</v>
-      </c>
-      <c r="F102">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G102" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B103" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="D103">
-        <v>3</v>
-      </c>
-      <c r="E103" t="s">
-        <v>169</v>
-      </c>
-      <c r="F103">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G103" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B104" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C104" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B105" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C105" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G105" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C106" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E106" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="F106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G106" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B107" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C107" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E107" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="F107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G107" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B108" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C108" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="F108">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G108" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B109" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C109" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D109">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F109">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B110" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C110" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F110">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G110" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B111" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C111" t="s">
         <v>198</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E111" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G111" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B112" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C112" t="s">
         <v>198</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E112" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F112">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G112" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B113" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C113" t="s">
         <v>198</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G113" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B114" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C114" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D114">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F114">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B115" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C115" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D115">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E115" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F115">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G115" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B116" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="C116" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E116" t="s">
+        <v>197</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
       </c>
       <c r="G116" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B117" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="C117" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="D117">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E117" t="s">
+        <v>197</v>
+      </c>
+      <c r="F117">
+        <v>4</v>
       </c>
       <c r="G117" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B118" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="C118" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="D118">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E118" t="s">
+        <v>197</v>
+      </c>
+      <c r="F118">
+        <v>5</v>
       </c>
       <c r="G118" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B119" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C119" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D119">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G119" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B120" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C120" t="s">
+        <v>154</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="G120" t="s">
         <v>156</v>
-      </c>
-      <c r="D120">
-        <v>5</v>
-      </c>
-      <c r="G120" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C121" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G121" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B122" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C122" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D122">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G122" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C123" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D123">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G123" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B124" t="s">
+        <v>147</v>
+      </c>
+      <c r="C124" t="s">
+        <v>148</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="G124" t="s">
         <v>149</v>
-      </c>
-      <c r="C124" t="s">
-        <v>150</v>
-      </c>
-      <c r="D124">
-        <v>4</v>
-      </c>
-      <c r="G124" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B125" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C125" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D125">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G125" t="s">
         <v>152</v>
@@ -3451,851 +3457,860 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B126" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C126" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126" t="s">
-        <v>169</v>
-      </c>
-      <c r="F126">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G126" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B127" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C127" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D127">
-        <v>2</v>
-      </c>
-      <c r="E127" t="s">
-        <v>169</v>
-      </c>
-      <c r="F127">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G127" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B128" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C128" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D128">
-        <v>3</v>
-      </c>
-      <c r="E128" t="s">
-        <v>169</v>
-      </c>
-      <c r="F128">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G128" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B129" t="s">
+        <v>166</v>
+      </c>
+      <c r="C129" t="s">
         <v>168</v>
       </c>
-      <c r="C129" t="s">
-        <v>170</v>
-      </c>
       <c r="D129">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F129">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B130" t="s">
+        <v>166</v>
+      </c>
+      <c r="C130" t="s">
         <v>168</v>
       </c>
-      <c r="C130" t="s">
-        <v>170</v>
-      </c>
       <c r="D130">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E130" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F130">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G130" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B131" t="s">
+        <v>166</v>
+      </c>
+      <c r="C131" t="s">
         <v>168</v>
       </c>
-      <c r="C131" t="s">
-        <v>180</v>
-      </c>
       <c r="D131">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E131" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F131">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G131" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B132" t="s">
+        <v>166</v>
+      </c>
+      <c r="C132" t="s">
         <v>168</v>
       </c>
-      <c r="C132" t="s">
-        <v>180</v>
-      </c>
       <c r="D132">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E132" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F132">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G132" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B133" t="s">
+        <v>166</v>
+      </c>
+      <c r="C133" t="s">
         <v>168</v>
       </c>
-      <c r="C133" t="s">
-        <v>180</v>
-      </c>
       <c r="D133">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E133" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F133">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G133" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C134" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D134">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E134" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F134">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C135" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D135">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E135" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F135">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G135" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="C136" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F136">
+        <v>3</v>
       </c>
       <c r="G136" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="C137" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E137" t="s">
+        <v>167</v>
+      </c>
+      <c r="F137">
+        <v>4</v>
       </c>
       <c r="G137" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="C138" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E138" t="s">
+        <v>167</v>
+      </c>
+      <c r="F138">
+        <v>5</v>
       </c>
       <c r="G138" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>136</v>
+      </c>
+      <c r="B139" t="s">
+        <v>137</v>
+      </c>
+      <c r="C139" t="s">
+        <v>139</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="G139" t="s">
         <v>138</v>
-      </c>
-      <c r="B139" t="s">
-        <v>139</v>
-      </c>
-      <c r="C139" t="s">
-        <v>141</v>
-      </c>
-      <c r="D139">
-        <v>3</v>
-      </c>
-      <c r="G139" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B140" t="s">
+        <v>137</v>
+      </c>
+      <c r="C140" t="s">
         <v>139</v>
       </c>
-      <c r="C140" t="s">
-        <v>141</v>
-      </c>
       <c r="D140">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G140" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B141" t="s">
+        <v>137</v>
+      </c>
+      <c r="C141" t="s">
         <v>139</v>
       </c>
-      <c r="C141" t="s">
-        <v>141</v>
-      </c>
       <c r="D141">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B142" t="s">
+        <v>137</v>
+      </c>
+      <c r="C142" t="s">
         <v>139</v>
       </c>
-      <c r="C142" t="s">
-        <v>148</v>
-      </c>
       <c r="D142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G142" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B143" t="s">
+        <v>137</v>
+      </c>
+      <c r="C143" t="s">
         <v>139</v>
       </c>
-      <c r="C143" t="s">
-        <v>148</v>
-      </c>
       <c r="D143">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G143" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B144" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C144" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G144" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B145" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C145" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="D145">
         <v>2</v>
       </c>
       <c r="G145" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B146" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C146" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="D146">
         <v>3</v>
       </c>
       <c r="G146" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B147" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C147" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D147">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B148" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C148" t="s">
+        <v>160</v>
+      </c>
+      <c r="D148">
+        <v>2</v>
+      </c>
+      <c r="G148" t="s">
         <v>162</v>
-      </c>
-      <c r="D148">
-        <v>5</v>
-      </c>
-      <c r="G148" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B149" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="E149" t="s">
-        <v>169</v>
-      </c>
-      <c r="F149">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G149" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B150" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C150" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D150">
-        <v>2</v>
-      </c>
-      <c r="E150" t="s">
-        <v>169</v>
-      </c>
-      <c r="F150">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G150" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B151" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C151" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D151">
-        <v>3</v>
-      </c>
-      <c r="E151" t="s">
-        <v>169</v>
-      </c>
-      <c r="F151">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G151" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B152" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C152" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D152">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F152">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G152" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B153" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C153" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D153">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F153">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G153" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B154" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="C154" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="D154">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E154" t="s">
+        <v>167</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
       </c>
       <c r="G154" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B155" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="C155" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="D155">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E155" t="s">
+        <v>167</v>
+      </c>
+      <c r="F155">
+        <v>4</v>
       </c>
       <c r="G155" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B156" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="C156" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="D156">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E156" t="s">
+        <v>167</v>
+      </c>
+      <c r="F156">
+        <v>5</v>
       </c>
       <c r="G156" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B157" t="s">
+        <v>210</v>
+      </c>
+      <c r="C157" t="s">
+        <v>211</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="G157" t="s">
         <v>212</v>
-      </c>
-      <c r="C157" t="s">
-        <v>213</v>
-      </c>
-      <c r="D157">
-        <v>4</v>
-      </c>
-      <c r="G157" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B158" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C158" t="s">
+        <v>211</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="G158" t="s">
         <v>213</v>
-      </c>
-      <c r="D158">
-        <v>5</v>
-      </c>
-      <c r="G158" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B159" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C159" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G159" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B160" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C160" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D160">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G160" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B161" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C161" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="D161">
-        <v>1</v>
-      </c>
-      <c r="E161" t="s">
-        <v>199</v>
-      </c>
-      <c r="F161">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G161" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B162" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C162" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D162">
-        <v>2</v>
-      </c>
-      <c r="E162" t="s">
-        <v>199</v>
-      </c>
-      <c r="F162">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G162" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B163" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C163" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D163">
         <v>3</v>
       </c>
-      <c r="E163" t="s">
-        <v>199</v>
-      </c>
-      <c r="F163">
-        <v>3</v>
-      </c>
       <c r="G163" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B164" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C164" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D164">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E164" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F164">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G164" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C165" t="s">
+        <v>199</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165" t="s">
+        <v>197</v>
+      </c>
+      <c r="F165">
+        <v>2</v>
+      </c>
+      <c r="G165" t="s">
         <v>201</v>
       </c>
-      <c r="D165">
-        <v>5</v>
-      </c>
-      <c r="E165" t="s">
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>136</v>
+      </c>
+      <c r="B166" t="s">
+        <v>166</v>
+      </c>
+      <c r="C166" t="s">
         <v>199</v>
       </c>
-      <c r="F165">
-        <v>5</v>
-      </c>
-      <c r="G165" t="s">
-        <v>206</v>
+      <c r="D166">
+        <v>3</v>
+      </c>
+      <c r="E166" t="s">
+        <v>197</v>
+      </c>
+      <c r="F166">
+        <v>3</v>
+      </c>
+      <c r="G166" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>136</v>
+      </c>
+      <c r="B167" t="s">
+        <v>166</v>
+      </c>
+      <c r="C167" t="s">
+        <v>199</v>
+      </c>
+      <c r="D167">
+        <v>4</v>
+      </c>
+      <c r="E167" t="s">
+        <v>197</v>
+      </c>
+      <c r="F167">
+        <v>4</v>
+      </c>
+      <c r="G167" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="B168" t="s">
-        <v>229</v>
+        <v>166</v>
       </c>
       <c r="C168" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="D168">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E168" t="s">
+        <v>197</v>
+      </c>
+      <c r="F168">
+        <v>5</v>
       </c>
       <c r="G168" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>89</v>
-      </c>
-      <c r="B169" t="s">
-        <v>232</v>
-      </c>
-      <c r="C169" t="s">
-        <v>233</v>
-      </c>
-      <c r="D169">
-        <v>5</v>
-      </c>
-      <c r="G169" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>89</v>
-      </c>
-      <c r="B170" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G174">
-    <sortCondition ref="A2:A174"/>
-    <sortCondition ref="C2:C174"/>
-    <sortCondition ref="D2:D174"/>
+  <sortState ref="A2:G171">
+    <sortCondition ref="A2:A171"/>
+    <sortCondition ref="C2:C171"/>
+    <sortCondition ref="D2:D171"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>